<commit_message>
#temp fixed antiforgery exception
</commit_message>
<xml_diff>
--- a/WorkHunter/WorkHunter.Api/Templates/WResponses/WResponsesTemplate.xlsx
+++ b/WorkHunter/WorkHunter.Api/Templates/WResponses/WResponsesTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funfo\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funfo\source\repos\work-hunter-helper\WorkHunter\WorkHunter.Api\Templates\WResponses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7798413-EEDB-4E01-BB83-2E9DFF1E1C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B880C2-F00D-4524-843B-BF1088576B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{63E05E47-4AE4-4823-8EAB-42D225B5043F}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{63E05E47-4AE4-4823-8EAB-42D225B5043F}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Status</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>https://testcompany/department/vacancy1</t>
+  </si>
+  <si>
+    <t>d6485221-63e8-42a0-9873-00622ec70e79</t>
   </si>
 </sst>
 </file>
@@ -225,6 +228,13 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,13 +244,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -592,62 +595,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -669,7 +672,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,48 +687,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -733,8 +736,8 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>22</v>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -742,16 +745,16 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#50 added wresponses export api
</commit_message>
<xml_diff>
--- a/WorkHunter/WorkHunter.Api/Templates/WResponses/WResponsesTemplate.xlsx
+++ b/WorkHunter/WorkHunter.Api/Templates/WResponses/WResponsesTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funfo\source\repos\work-hunter-helper\WorkHunter\WorkHunter.Api\Templates\WResponses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B880C2-F00D-4524-843B-BF1088576B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B5CD4A-B033-41B0-9194-1A296EEE0788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{63E05E47-4AE4-4823-8EAB-42D225B5043F}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="597" xr2:uid="{63E05E47-4AE4-4823-8EAB-42D225B5043F}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Status</t>
   </si>
@@ -81,73 +81,20 @@
     <t>Password</t>
   </si>
   <si>
-    <t>User 1</t>
-  </si>
-  <si>
-    <t>user1@test.com</t>
-  </si>
-  <si>
-    <t>user1uycv632409@test.com</t>
-  </si>
-  <si>
-    <t>Q1_s68sjdbkj</t>
-  </si>
-  <si>
-    <t>user2uycv632409@test.com</t>
-  </si>
-  <si>
-    <t>user2@test.com</t>
-  </si>
-  <si>
-    <t>Q2_s68sjdbkj</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
-    <t>d6485221-65g8-42a0-9873-00622ec70e79</t>
-  </si>
-  <si>
-    <t>d6485221-98g8-42a0-9873-00622ec70e79</t>
-  </si>
-  <si>
-    <t>User 2</t>
-  </si>
-  <si>
     <t>Users</t>
-  </si>
-  <si>
-    <t>+7 __________</t>
-  </si>
-  <si>
-    <t>Rejected (without text by timeout)</t>
-  </si>
-  <si>
-    <t>testcompany@test.com</t>
-  </si>
-  <si>
-    <t>https://testcompany/department/vacancy1</t>
-  </si>
-  <si>
-    <t>d6485221-63e8-42a0-9873-00622ec70e79</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,16 +169,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,8 +188,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -579,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF037E0-1F57-4F55-AE53-E9DEDAD404D3}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,17 +537,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -618,61 +560,22 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{44F192BF-BBD8-41B4-9A09-DD4AED1B5DF3}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{EFA82323-32B8-4DAD-B38F-E8FDBAA02F91}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{6A24A066-9B11-4C7F-B27D-18F7D8E78A75}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178E47E8-A499-43D0-9789-9FD19BCA33A1}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,18 +590,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -730,43 +633,13 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{C14E1D4D-0803-475D-B30F-D2BABF35B85D}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{4A704C4C-15D9-4BA8-AA97-72A650B93BF5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>